<commit_message>
parse column last year get ki quater A,D
</commit_message>
<xml_diff>
--- a/2021.01.08 Ki Quy 3 2020 Gen - Dieu chinh danh sach New Format.xlsx
+++ b/2021.01.08 Ki Quy 3 2020 Gen - Dieu chinh danh sach New Format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TT HTDT-DK\Danh gia Ki\Ki 2020\Quy 4 2020\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$5:$AK$58</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -510,7 +510,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -890,13 +890,13 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1497,8 +1497,8 @@
   </sheetPr>
   <dimension ref="A4:AK61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AK7" sqref="AK7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,7 +1547,7 @@
       <c r="AF4" s="4"/>
     </row>
     <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="65" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="64" t="s">
@@ -1565,48 +1565,56 @@
       <c r="F5" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="65" t="s">
+      <c r="G5" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65" t="s">
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="65" t="s">
+      <c r="K5" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65" t="s">
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="65" t="s">
+      <c r="O5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="65"/>
-      <c r="R5" s="65" t="s">
+      <c r="P5" s="63"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="65" t="s">
+      <c r="S5" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="65"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65" t="s">
+      <c r="T5" s="63"/>
+      <c r="U5" s="63"/>
+      <c r="V5" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="W5" s="65" t="s">
+      <c r="W5" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="X5" s="65" t="s">
+      <c r="X5" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
+      <c r="Y5" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>3</v>
+      </c>
       <c r="AC5" s="5"/>
       <c r="AD5" s="5"/>
       <c r="AE5" s="5"/>
@@ -1614,7 +1622,7 @@
       <c r="AG5" s="58"/>
     </row>
     <row r="6" spans="1:37" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="63"/>
+      <c r="A6" s="65"/>
       <c r="B6" s="64"/>
       <c r="C6" s="64"/>
       <c r="D6" s="64"/>
@@ -1629,7 +1637,7 @@
       <c r="I6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="65"/>
+      <c r="J6" s="63"/>
       <c r="K6" s="6" t="s">
         <v>18</v>
       </c>
@@ -1639,7 +1647,7 @@
       <c r="M6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="65"/>
+      <c r="N6" s="63"/>
       <c r="O6" s="6" t="s">
         <v>21</v>
       </c>
@@ -1649,7 +1657,7 @@
       <c r="Q6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="R6" s="65"/>
+      <c r="R6" s="63"/>
       <c r="S6" s="6" t="s">
         <v>24</v>
       </c>
@@ -1659,9 +1667,9 @@
       <c r="U6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="V6" s="65"/>
-      <c r="W6" s="65"/>
-      <c r="X6" s="65"/>
+      <c r="V6" s="63"/>
+      <c r="W6" s="63"/>
+      <c r="X6" s="63"/>
       <c r="Y6" s="7" t="s">
         <v>27</v>
       </c>
@@ -1826,6 +1834,12 @@
         <v>0</v>
       </c>
       <c r="AG8" s="56"/>
+      <c r="AH8">
+        <v>2018</v>
+      </c>
+      <c r="AI8">
+        <v>2019</v>
+      </c>
     </row>
     <row r="9" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
@@ -1876,6 +1890,12 @@
       <c r="AG9" s="57">
         <v>1</v>
       </c>
+      <c r="AH9">
+        <v>2018</v>
+      </c>
+      <c r="AI9">
+        <v>2019</v>
+      </c>
     </row>
     <row r="10" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
@@ -1967,6 +1987,12 @@
         <v>0</v>
       </c>
       <c r="AG10" s="56"/>
+      <c r="AH10">
+        <v>2018</v>
+      </c>
+      <c r="AI10">
+        <v>2019</v>
+      </c>
     </row>
     <row r="11" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
@@ -2060,6 +2086,12 @@
       <c r="AG11" s="56">
         <v>1</v>
       </c>
+      <c r="AH11">
+        <v>2018</v>
+      </c>
+      <c r="AI11">
+        <v>2019</v>
+      </c>
     </row>
     <row r="12" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
@@ -2151,6 +2183,12 @@
         <v>1</v>
       </c>
       <c r="AG12" s="56"/>
+      <c r="AH12">
+        <v>2017</v>
+      </c>
+      <c r="AI12">
+        <v>2019</v>
+      </c>
     </row>
     <row r="13" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
@@ -2242,6 +2280,12 @@
         <v>0</v>
       </c>
       <c r="AG13" s="56"/>
+      <c r="AH13">
+        <v>2017</v>
+      </c>
+      <c r="AI13">
+        <v>2018</v>
+      </c>
     </row>
     <row r="14" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
@@ -2333,6 +2377,12 @@
         <v>1</v>
       </c>
       <c r="AG14" s="56"/>
+      <c r="AH14">
+        <v>2017</v>
+      </c>
+      <c r="AI14">
+        <v>2018</v>
+      </c>
     </row>
     <row r="15" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
@@ -2424,6 +2474,12 @@
         <v>1</v>
       </c>
       <c r="AG15" s="56"/>
+      <c r="AH15">
+        <v>2018</v>
+      </c>
+      <c r="AI15">
+        <v>2018</v>
+      </c>
     </row>
     <row r="16" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
@@ -2515,8 +2571,14 @@
         <v>0</v>
       </c>
       <c r="AG16" s="56"/>
+      <c r="AH16">
+        <v>2018</v>
+      </c>
+      <c r="AI16">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="17" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2606,8 +2668,14 @@
         <v>1</v>
       </c>
       <c r="AG17" s="56"/>
+      <c r="AH17">
+        <v>2018</v>
+      </c>
+      <c r="AI17">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="18" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2697,8 +2765,14 @@
         <v>0</v>
       </c>
       <c r="AG18" s="56"/>
+      <c r="AH18">
+        <v>2018</v>
+      </c>
+      <c r="AI18">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="19" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2788,8 +2862,14 @@
         <v>1</v>
       </c>
       <c r="AG19" s="56"/>
+      <c r="AH19">
+        <v>2019</v>
+      </c>
+      <c r="AI19">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="20" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2879,8 +2959,14 @@
         <v>1</v>
       </c>
       <c r="AG20" s="56"/>
+      <c r="AH20">
+        <v>2019</v>
+      </c>
+      <c r="AI20">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="21" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2970,8 +3056,14 @@
         <v>1</v>
       </c>
       <c r="AG21" s="56"/>
+      <c r="AH21">
+        <v>2019</v>
+      </c>
+      <c r="AI21">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="22" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3061,8 +3153,14 @@
         <v>1</v>
       </c>
       <c r="AG22" s="56"/>
+      <c r="AH22">
+        <v>2019</v>
+      </c>
+      <c r="AI22">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="23" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3152,8 +3250,14 @@
         <v>0</v>
       </c>
       <c r="AG23" s="56"/>
+      <c r="AH23">
+        <v>2018</v>
+      </c>
+      <c r="AI23">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="24" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3243,8 +3347,14 @@
         <v>1</v>
       </c>
       <c r="AG24" s="56"/>
+      <c r="AH24">
+        <v>2018</v>
+      </c>
+      <c r="AI24">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="25" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3330,8 +3440,14 @@
         <v>0</v>
       </c>
       <c r="AG25" s="56"/>
+      <c r="AH25">
+        <v>2020</v>
+      </c>
+      <c r="AI25">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="26" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3421,8 +3537,14 @@
         <v>1</v>
       </c>
       <c r="AG26" s="56"/>
+      <c r="AH26">
+        <v>2020</v>
+      </c>
+      <c r="AI26">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="27" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="18">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3512,8 +3634,14 @@
         <v>0</v>
       </c>
       <c r="AG27" s="56"/>
+      <c r="AH27">
+        <v>2020</v>
+      </c>
+      <c r="AI27">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="28" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3603,8 +3731,14 @@
         <v>1</v>
       </c>
       <c r="AG28" s="56"/>
+      <c r="AH28">
+        <v>2020</v>
+      </c>
+      <c r="AI28">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="29" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="18">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3694,8 +3828,14 @@
         <v>0</v>
       </c>
       <c r="AG29" s="56"/>
+      <c r="AH29">
+        <v>2018</v>
+      </c>
+      <c r="AI29">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="30" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3785,8 +3925,14 @@
         <v>0</v>
       </c>
       <c r="AG30" s="56"/>
+      <c r="AH30">
+        <v>2018</v>
+      </c>
+      <c r="AI30">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="31" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="18">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3876,8 +4022,14 @@
         <v>1</v>
       </c>
       <c r="AG31" s="56"/>
+      <c r="AH31">
+        <v>2018</v>
+      </c>
+      <c r="AI31">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="32" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="18">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3963,8 +4115,14 @@
         <v>1</v>
       </c>
       <c r="AG32" s="56"/>
+      <c r="AH32">
+        <v>2018</v>
+      </c>
+      <c r="AI32">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="33" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="18">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4054,8 +4212,14 @@
         <v>1</v>
       </c>
       <c r="AG33" s="56"/>
+      <c r="AH33">
+        <v>2018</v>
+      </c>
+      <c r="AI33">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="34" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="18">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4145,8 +4309,14 @@
         <v>1</v>
       </c>
       <c r="AG34" s="56"/>
+      <c r="AH34">
+        <v>2018</v>
+      </c>
+      <c r="AI34">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="35" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="18">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4236,8 +4406,14 @@
         <v>0</v>
       </c>
       <c r="AG35" s="56"/>
+      <c r="AH35">
+        <v>2018</v>
+      </c>
+      <c r="AI35">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="36" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="18">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4327,8 +4503,14 @@
         <v>1</v>
       </c>
       <c r="AG36" s="56"/>
+      <c r="AH36">
+        <v>2018</v>
+      </c>
+      <c r="AI36">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="37" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="18">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4418,8 +4600,14 @@
         <v>1</v>
       </c>
       <c r="AG37" s="56"/>
+      <c r="AH37">
+        <v>2018</v>
+      </c>
+      <c r="AI37">
+        <v>2019</v>
+      </c>
     </row>
-    <row r="38" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="18">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -4505,8 +4693,14 @@
         <v>1</v>
       </c>
       <c r="AG38" s="56"/>
+      <c r="AH38">
+        <v>2018</v>
+      </c>
+      <c r="AI38">
+        <v>2019</v>
+      </c>
     </row>
-    <row r="39" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="18">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -4592,8 +4786,14 @@
         <v>0</v>
       </c>
       <c r="AG39" s="56"/>
+      <c r="AH39">
+        <v>2018</v>
+      </c>
+      <c r="AI39">
+        <v>2019</v>
+      </c>
     </row>
-    <row r="40" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="18">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -4679,8 +4879,14 @@
         <v>1</v>
       </c>
       <c r="AG40" s="56"/>
+      <c r="AH40">
+        <v>2018</v>
+      </c>
+      <c r="AI40">
+        <v>2019</v>
+      </c>
     </row>
-    <row r="41" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="18">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -4766,8 +4972,14 @@
         <v>0</v>
       </c>
       <c r="AG41" s="56"/>
+      <c r="AH41">
+        <v>2019</v>
+      </c>
+      <c r="AI41">
+        <v>2019</v>
+      </c>
     </row>
-    <row r="42" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="18">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -4853,8 +5065,14 @@
         <v>1</v>
       </c>
       <c r="AG42" s="56"/>
+      <c r="AH42">
+        <v>2019</v>
+      </c>
+      <c r="AI42">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="43" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="18">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -4940,8 +5158,14 @@
         <v>1</v>
       </c>
       <c r="AG43" s="56"/>
+      <c r="AH43">
+        <v>2019</v>
+      </c>
+      <c r="AI43">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="44" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="18">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -5027,8 +5251,14 @@
         <v>0</v>
       </c>
       <c r="AG44" s="56"/>
+      <c r="AH44">
+        <v>2019</v>
+      </c>
+      <c r="AI44">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="45" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="18">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -5114,8 +5344,14 @@
         <v>1</v>
       </c>
       <c r="AG45" s="56"/>
+      <c r="AH45">
+        <v>2019</v>
+      </c>
+      <c r="AI45">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="46" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="18">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -5201,8 +5437,14 @@
         <v>1</v>
       </c>
       <c r="AG46" s="56"/>
+      <c r="AH46">
+        <v>2018</v>
+      </c>
+      <c r="AI46">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="47" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="18">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -5288,8 +5530,14 @@
         <v>1</v>
       </c>
       <c r="AG47" s="56"/>
+      <c r="AH47">
+        <v>2018</v>
+      </c>
+      <c r="AI47">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="48" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="18">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -5375,8 +5623,14 @@
         <v>0</v>
       </c>
       <c r="AG48" s="56"/>
+      <c r="AH48">
+        <v>2018</v>
+      </c>
+      <c r="AI48">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="49" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="18">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -5462,8 +5716,14 @@
         <v>1</v>
       </c>
       <c r="AG49" s="56"/>
+      <c r="AH49">
+        <v>2018</v>
+      </c>
+      <c r="AI49">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="50" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="18">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -5549,8 +5809,14 @@
         <v>0</v>
       </c>
       <c r="AG50" s="56"/>
+      <c r="AH50">
+        <v>2018</v>
+      </c>
+      <c r="AI50">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="51" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="18">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -5636,8 +5902,14 @@
         <v>0</v>
       </c>
       <c r="AG51" s="56"/>
+      <c r="AH51">
+        <v>2018</v>
+      </c>
+      <c r="AI51">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="52" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="18">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -5723,8 +5995,14 @@
         <v>1</v>
       </c>
       <c r="AG52" s="56"/>
+      <c r="AH52">
+        <v>2018</v>
+      </c>
+      <c r="AI52">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="53" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="18">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -5810,8 +6088,14 @@
         <v>0</v>
       </c>
       <c r="AG53" s="56"/>
+      <c r="AH53">
+        <v>2018</v>
+      </c>
+      <c r="AI53">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="54" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="18">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -5897,8 +6181,14 @@
         <v>1</v>
       </c>
       <c r="AG54" s="56"/>
+      <c r="AH54">
+        <v>2020</v>
+      </c>
+      <c r="AI54">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="55" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="18">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -5986,8 +6276,14 @@
         <v>0</v>
       </c>
       <c r="AG55" s="56"/>
+      <c r="AH55">
+        <v>2020</v>
+      </c>
+      <c r="AI55">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="56" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="18">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -6075,8 +6371,14 @@
         <v>0</v>
       </c>
       <c r="AG56" s="56"/>
+      <c r="AH56">
+        <v>2020</v>
+      </c>
+      <c r="AI56">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="57" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="18">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -6156,8 +6458,14 @@
         <v>0</v>
       </c>
       <c r="AG57" s="56"/>
+      <c r="AH57">
+        <v>2020</v>
+      </c>
+      <c r="AI57">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="58" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="18">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -6237,8 +6545,14 @@
         <v>0</v>
       </c>
       <c r="AG58" s="56"/>
+      <c r="AH58">
+        <v>2018</v>
+      </c>
+      <c r="AI58">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="59" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="18">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -6307,8 +6621,14 @@
         <v>0</v>
       </c>
       <c r="AG59" s="56"/>
+      <c r="AH59">
+        <v>2018</v>
+      </c>
+      <c r="AI59">
+        <v>2019</v>
+      </c>
     </row>
-    <row r="60" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="18">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -6369,8 +6689,14 @@
         <v>0</v>
       </c>
       <c r="AG60" s="56"/>
+      <c r="AH60">
+        <v>2018</v>
+      </c>
+      <c r="AI60">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="61" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="18">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -6431,25 +6757,31 @@
         <v>0</v>
       </c>
       <c r="AG61" s="56"/>
+      <c r="AH61">
+        <v>2018</v>
+      </c>
+      <c r="AI61">
+        <v>2018</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:N6"/>
     <mergeCell ref="X5:X6"/>
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="R5:R6"/>
     <mergeCell ref="S5:U5"/>
     <mergeCell ref="V5:V6"/>
     <mergeCell ref="W5:W6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="G8:W45">
     <cfRule type="cellIs" priority="53" operator="equal">

</xml_diff>